<commit_message>
excel plots - third part
</commit_message>
<xml_diff>
--- a/results/sixth1.xlsx
+++ b/results/sixth1.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pawel\IdeaProjects\TinyGP\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\IdeaProjects\TinyGP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D54D005-E604-4790-98EB-2514E87257FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19068EB9-E929-41ED-BC51-C750C5F87DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="1170" windowWidth="45780" windowHeight="16410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TinyGP" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
   <si>
     <t>X1</t>
   </si>
@@ -344,6 +344,18 @@
   <si>
     <t>Gen 99 best individual</t>
   </si>
+  <si>
+    <t>Gen 0</t>
+  </si>
+  <si>
+    <t>Gen 11</t>
+  </si>
+  <si>
+    <t>Gen 50</t>
+  </si>
+  <si>
+    <t>Gen 99</t>
+  </si>
 </sst>
 </file>
 
@@ -378,8 +390,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -395,6 +410,316 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>291678</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E84690E5-D5E5-2585-9617-F29E8020F691}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="209550" y="609600"/>
+          <a:ext cx="3739728" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>69849</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Obraz 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56D0C9FA-B6C5-B15E-9AB9-0AA06044D6FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5048250" y="740440"/>
+          <a:ext cx="3714750" cy="2459959"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>508348</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obraz 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9F44AF-1D5B-D488-BE0B-E184A1435C96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="311150" y="3949700"/>
+          <a:ext cx="3854798" cy="2552700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>34294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Obraz 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41C24956-EE70-FA8F-CF14-024E21A99ECD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5207000" y="3901444"/>
+          <a:ext cx="3898900" cy="2581905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>349249</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>224518</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Obraz 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5372E8D0-ACFA-C59E-ECE8-F96B8D6C42F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="349249" y="7581900"/>
+          <a:ext cx="4142469" cy="2743200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,17 +1021,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CY101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CG64" workbookViewId="0">
-      <selection activeCell="CU80" sqref="CU80"/>
+    <sheetView topLeftCell="CE1" workbookViewId="0">
+      <selection activeCell="CH17" sqref="CH17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15.5703125" customWidth="1"/>
-    <col min="4" max="103" width="23.42578125" customWidth="1"/>
+    <col min="1" max="2" width="15.54296875" customWidth="1"/>
+    <col min="4" max="103" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1017,7 +1342,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>-0.54</v>
       </c>
@@ -1424,7 +1749,7 @@
         <v>46.718999784233297</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>-4.51</v>
       </c>
@@ -1831,7 +2156,7 @@
         <v>-55.236799968175696</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>-3.57</v>
       </c>
@@ -2238,7 +2563,7 @@
         <v>24.547999260449764</v>
       </c>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>9.15</v>
       </c>
@@ -2645,7 +2970,7 @@
         <v>-17.527500397279329</v>
       </c>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>-8.7899999999999991</v>
       </c>
@@ -3052,7 +3377,7 @@
         <v>249.45219960819017</v>
       </c>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3.62</v>
       </c>
@@ -3459,7 +3784,7 @@
         <v>9.7425990409744898</v>
       </c>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>-7.94</v>
       </c>
@@ -3866,7 +4191,7 @@
         <v>97.020999190507069</v>
       </c>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9.84</v>
       </c>
@@ -4273,7 +4598,7 @@
         <v>166.73679987508038</v>
       </c>
     </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>-6.68</v>
       </c>
@@ -4680,7 +5005,7 @@
         <v>140.53279891720956</v>
       </c>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2.16</v>
       </c>
@@ -5087,7 +5412,7 @@
         <v>7.3763988761969994</v>
       </c>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>-4.21</v>
       </c>
@@ -5494,7 +5819,7 @@
         <v>-43.699300201331141</v>
       </c>
     </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.96</v>
       </c>
@@ -5901,7 +6226,7 @@
         <v>40.402404380934783</v>
       </c>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.08</v>
       </c>
@@ -6308,7 +6633,7 @@
         <v>-60.644800063408908</v>
       </c>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>-7.73</v>
       </c>
@@ -6715,7 +7040,7 @@
         <v>195.40029923395443</v>
       </c>
     </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>-2.7</v>
       </c>
@@ -7122,7 +7447,7 @@
         <v>127.73100196128699</v>
       </c>
     </row>
-    <row r="17" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>-0.06</v>
       </c>
@@ -7529,7 +7854,7 @@
         <v>57.438402114817066</v>
       </c>
     </row>
-    <row r="18" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2.19</v>
       </c>
@@ -7936,7 +8261,7 @@
         <v>3.0139993545498065</v>
       </c>
     </row>
-    <row r="19" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>9.1999999999999993</v>
       </c>
@@ -8343,7 +8668,7 @@
         <v>-46.199999409044949</v>
       </c>
     </row>
-    <row r="20" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5.81</v>
       </c>
@@ -8750,7 +9075,7 @@
         <v>62.604200083620768</v>
       </c>
     </row>
-    <row r="21" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>9.01</v>
       </c>
@@ -9157,7 +9482,7 @@
         <v>-62.236198888736858</v>
       </c>
     </row>
-    <row r="22" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>8.7200000000000006</v>
       </c>
@@ -9564,7 +9889,7 @@
         <v>-104.78999535144209</v>
       </c>
     </row>
-    <row r="23" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>-5.52</v>
       </c>
@@ -9971,7 +10296,7 @@
         <v>94.846799060287196</v>
       </c>
     </row>
-    <row r="24" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>-6.1</v>
       </c>
@@ -10378,7 +10703,7 @@
         <v>-96.133000520513349</v>
       </c>
     </row>
-    <row r="25" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8.3800000000000008</v>
       </c>
@@ -10785,7 +11110,7 @@
         <v>250.0848004910525</v>
       </c>
     </row>
-    <row r="26" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>-5.67</v>
       </c>
@@ -11192,7 +11517,7 @@
         <v>9.8591997436806054</v>
       </c>
     </row>
-    <row r="27" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>-2.08</v>
       </c>
@@ -11599,7 +11924,7 @@
         <v>60.669599173390203</v>
       </c>
     </row>
-    <row r="28" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>-0.16</v>
       </c>
@@ -12006,7 +12331,7 @@
         <v>-58.590000483598239</v>
       </c>
     </row>
-    <row r="29" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>4.1900000000000004</v>
       </c>
@@ -12413,7 +12738,7 @@
         <v>55.318099456112506</v>
       </c>
     </row>
-    <row r="30" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>-2.1800000000000002</v>
       </c>
@@ -12820,7 +13145,7 @@
         <v>-64.114000476887881</v>
       </c>
     </row>
-    <row r="31" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>-9.7100000000000009</v>
       </c>
@@ -13227,7 +13552,7 @@
         <v>412.86680342944521</v>
       </c>
     </row>
-    <row r="32" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>4.45</v>
       </c>
@@ -13634,7 +13959,7 @@
         <v>47.281999924350281</v>
       </c>
     </row>
-    <row r="33" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>6.91</v>
       </c>
@@ -14041,7 +14366,7 @@
         <v>21.15079902999225</v>
       </c>
     </row>
-    <row r="34" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>5.13</v>
       </c>
@@ -14448,7 +14773,7 @@
         <v>8.5232989634030343</v>
       </c>
     </row>
-    <row r="35" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.75</v>
       </c>
@@ -14855,7 +15180,7 @@
         <v>21.17999901824933</v>
       </c>
     </row>
-    <row r="36" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>5.0999999999999996</v>
       </c>
@@ -15262,7 +15587,7 @@
         <v>36.471999761462328</v>
       </c>
     </row>
-    <row r="37" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>5.44</v>
       </c>
@@ -15669,7 +15994,7 @@
         <v>65.357199938418972</v>
       </c>
     </row>
-    <row r="38" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0</v>
       </c>
@@ -16076,7 +16401,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>-8.69</v>
       </c>
@@ -16483,7 +16808,7 @@
         <v>15.336599930454087</v>
       </c>
     </row>
-    <row r="40" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>6.81</v>
       </c>
@@ -16890,7 +17215,7 @@
         <v>21.456199189304304</v>
       </c>
     </row>
-    <row r="41" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>-3.39</v>
       </c>
@@ -17297,7 +17622,7 @@
         <v>173.0316044567551</v>
       </c>
     </row>
-    <row r="42" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>6.7</v>
       </c>
@@ -17704,7 +18029,7 @@
         <v>99.992999892700738</v>
       </c>
     </row>
-    <row r="43" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>-3.16</v>
       </c>
@@ -18111,7 +18436,7 @@
         <v>155.3504032098698</v>
       </c>
     </row>
-    <row r="44" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>8.24</v>
       </c>
@@ -18518,7 +18843,7 @@
         <v>167.06639986935727</v>
       </c>
     </row>
-    <row r="45" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>-3.37</v>
       </c>
@@ -18925,7 +19250,7 @@
         <v>-46.159299923337237</v>
       </c>
     </row>
-    <row r="46" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.26</v>
       </c>
@@ -19332,7 +19657,7 @@
         <v>-21.822000203975641</v>
       </c>
     </row>
-    <row r="47" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>-5.57</v>
       </c>
@@ -19739,7 +20064,7 @@
         <v>-41.950300125132912</v>
       </c>
     </row>
-    <row r="48" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>8.61</v>
       </c>
@@ -20146,7 +20471,7 @@
         <v>-70.047198193821146</v>
       </c>
     </row>
-    <row r="49" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>-4.32</v>
       </c>
@@ -20553,7 +20878,7 @@
         <v>110.2807993402881</v>
       </c>
     </row>
-    <row r="50" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2.87</v>
       </c>
@@ -20960,7 +21285,7 @@
         <v>9.5106004746864343</v>
       </c>
     </row>
-    <row r="51" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1.32</v>
       </c>
@@ -21367,7 +21692,7 @@
         <v>1.1920000322526456</v>
       </c>
     </row>
-    <row r="52" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>-3.78</v>
       </c>
@@ -21774,7 +22099,7 @@
         <v>-25.609800134514067</v>
       </c>
     </row>
-    <row r="53" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>-5.0999999999999996</v>
       </c>
@@ -22181,7 +22506,7 @@
         <v>-31.416000180865023</v>
       </c>
     </row>
-    <row r="54" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>-6.86</v>
       </c>
@@ -22588,7 +22913,7 @@
         <v>305.10520435320126</v>
       </c>
     </row>
-    <row r="55" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>-9.57</v>
       </c>
@@ -22995,7 +23320,7 @@
         <v>397.19120284441493</v>
       </c>
     </row>
-    <row r="56" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2.33</v>
       </c>
@@ -23402,7 +23727,7 @@
         <v>6.4879001364912714</v>
       </c>
     </row>
-    <row r="57" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>-7.51</v>
       </c>
@@ -23809,7 +24134,7 @@
         <v>237.82840010058464</v>
       </c>
     </row>
-    <row r="58" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>-4.5999999999999996</v>
       </c>
@@ -24216,7 +24541,7 @@
         <v>180.65600164220123</v>
       </c>
     </row>
-    <row r="59" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>-2.25</v>
       </c>
@@ -24623,7 +24948,7 @@
         <v>-3.7000002446923919</v>
       </c>
     </row>
-    <row r="60" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>-1.56</v>
       </c>
@@ -25030,7 +25355,7 @@
         <v>-56.017600109958849</v>
       </c>
     </row>
-    <row r="61" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>6.01</v>
       </c>
@@ -25437,7 +25762,7 @@
         <v>5.3536988692375065</v>
       </c>
     </row>
-    <row r="62" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>9.99</v>
       </c>
@@ -25844,7 +26169,7 @@
         <v>109.06929987758838</v>
       </c>
     </row>
-    <row r="63" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>3.28</v>
       </c>
@@ -26251,7 +26576,7 @@
         <v>32.035999608837514</v>
       </c>
     </row>
-    <row r="64" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>6.73</v>
       </c>
@@ -26658,7 +26983,7 @@
         <v>-51.972598425520466</v>
       </c>
     </row>
-    <row r="65" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>-7.54</v>
       </c>
@@ -26997,7 +27322,7 @@
         <v>#NUM!</v>
       </c>
       <c r="CH65" t="e">
-        <f t="shared" si="181"/>
+        <f>0.387793625346044+A65^E82-7.00000687341426*B65+3*A65*B65-0.373851905116872*(-1.80432696866735-SIN(0.410835718453507-COS(COS(COS(5.02949249135435+(-0.00219665917718252-6.45092198133839*B65)/(-0.99605525774826-0.805646271445614/(-3.22441378084339-3.22441378084339*(2.33764190756108-0.345147563289541*(-6.45092198133839-B65)-7.27494841459542*B65-0.0661693064893468*SIN(0.408363607696136-A65)-0.224887704476087*(-5.24203988703963-SIN(A65+3.22441378084339*B65*(2.39689207545382-A65*B65)))+3.22441378084339*B65*(1.99553339241374-A65+0.383158611593658*SIN(COS(A65)))))-1.0319084349848*B65*(1.53201274112214+2*B65+SIN(A65)-4.32745802431316*(182.79452071823-1.34325214910098*B65-SIN(6.45092198133839+0.426757316912592*(-3.98807269145233-SIN(6.45092198133839*(-2.63793400115128+A65))))))-SIN(COS(0.487137040773325*(6.82463230939217+SIN(12.199026455278*(-2.25186912174829-5.02949249135435*A65-3.22441378084339*(3.44942383085936-A65)*B65-0.485613365074091/(-2.48424598632624-A65^2+(-0.146734135347126+A65)*(1.73462548958879+A65)*B65)+4.11532584964218*(2.39689207545382-A65-0.292709528606689/COS(1.99553339241374-2.53138327426523*(A65+COS(2.63793400115128*A65)-0.485613365074091/(-0.272314227545209-SIN(6.59765611668551-A65^2-74.5667692216525*B65)))))+SIN(6.74876622178565+B65^2*(-6.80150622545258+SIN((0.875246077757794*(0.950678391751565*(-2.39689207545382+A65)+A65^2+A65*B65+2.48424598632624*(12.4765493570293+B65)-SIN(A65)))/(-1.07340769357997+SIN(3.66049616563898*B65^2)))))))))-(-0.146734135347126+4.24322024085258*(2.34325214910098-A65))*B65*(14.2776161951164+A65^2-6.03578708089649*B65+A65*B65-(-0.620893301029971-A65^2-0.345147563289541*(-2.53138327426523-B65)+3.22441378084339*(2.29688328766935-A65)*B65)*(27.7880884023096-B65-0.785586887684844*(-67.9880809247166-A65)*B65^2)-0.373851905116872*(2.95209955329819+COS(B65)-SIN(14.2424290222517+0.57538369517443*(-1.47555350471373-SIN(7.27494841459542*(4.05592028470151+0.643508579890146*A65))+SIN(3.66049616563898*B65^2))))))))))))</f>
         <v>#NUM!</v>
       </c>
       <c r="CI65" t="e">
@@ -27065,7 +27390,7 @@
         <v>337.46440437349258</v>
       </c>
     </row>
-    <row r="66" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>3.52</v>
       </c>
@@ -27472,7 +27797,7 @@
         <v>39.057999441787111</v>
       </c>
     </row>
-    <row r="67" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>0.53</v>
       </c>
@@ -27879,7 +28204,7 @@
         <v>-28.474100227688314</v>
       </c>
     </row>
-    <row r="68" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>4.47</v>
       </c>
@@ -28286,7 +28611,7 @@
         <v>2.7123990461635952</v>
       </c>
     </row>
-    <row r="69" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1.07</v>
       </c>
@@ -28693,7 +29018,7 @@
         <v>-20.746700524546544</v>
       </c>
     </row>
-    <row r="70" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>-5.14</v>
       </c>
@@ -29100,7 +29425,7 @@
         <v>223.14620315022742</v>
       </c>
     </row>
-    <row r="71" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>6.39</v>
       </c>
@@ -29507,7 +29832,7 @@
         <v>-12.32440067924275</v>
       </c>
     </row>
-    <row r="72" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>3.36</v>
       </c>
@@ -29914,7 +30239,7 @@
         <v>30.923599796461684</v>
       </c>
     </row>
-    <row r="73" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1.44</v>
       </c>
@@ -30321,7 +30646,7 @@
         <v>-6.1187998396065311</v>
       </c>
     </row>
-    <row r="74" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>5.42</v>
       </c>
@@ -30728,7 +31053,7 @@
         <v>57.230400051167486</v>
       </c>
     </row>
-    <row r="75" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>0.34</v>
       </c>
@@ -31135,7 +31460,7 @@
         <v>-57.428599465906494</v>
       </c>
     </row>
-    <row r="76" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2.42</v>
       </c>
@@ -31542,7 +31867,7 @@
         <v>7.5272001941129636</v>
       </c>
     </row>
-    <row r="77" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>2.95</v>
       </c>
@@ -31949,7 +32274,7 @@
         <v>-7.4284957940247134</v>
       </c>
     </row>
-    <row r="78" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>9.2799999999999994</v>
       </c>
@@ -32356,7 +32681,7 @@
         <v>179.85639997357455</v>
       </c>
     </row>
-    <row r="79" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1.1200000000000001</v>
       </c>
@@ -32763,7 +33088,7 @@
         <v>-22.64320068463137</v>
       </c>
     </row>
-    <row r="80" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>7.02</v>
       </c>
@@ -33170,7 +33495,7 @@
         <v>-72.744596815382593</v>
       </c>
     </row>
-    <row r="81" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>8.02</v>
       </c>
@@ -33577,7 +33902,7 @@
         <v>231.48480022126682</v>
       </c>
     </row>
-    <row r="82" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>7.35</v>
       </c>
@@ -33984,7 +34309,7 @@
         <v>91.142500099204497</v>
       </c>
     </row>
-    <row r="83" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>0.52</v>
       </c>
@@ -34391,7 +34716,7 @@
         <v>-40.182400326463537</v>
       </c>
     </row>
-    <row r="84" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>-3.67</v>
       </c>
@@ -34798,7 +35123,7 @@
         <v>-20.290400193674852</v>
       </c>
     </row>
-    <row r="85" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1.9</v>
       </c>
@@ -35205,7 +35530,7 @@
         <v>-0.10899997293788266</v>
       </c>
     </row>
-    <row r="86" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>-2.78</v>
       </c>
@@ -35612,7 +35937,7 @@
         <v>-41.126600202737002</v>
       </c>
     </row>
-    <row r="87" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>-2.2599999999999998</v>
       </c>
@@ -36019,7 +36344,7 @@
         <v>59.022798953111526</v>
       </c>
     </row>
-    <row r="88" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1.03</v>
       </c>
@@ -36426,7 +36751,7 @@
         <v>-0.55880008063365294</v>
       </c>
     </row>
-    <row r="89" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>-2.2200000000000002</v>
       </c>
@@ -36833,7 +37158,7 @@
         <v>-107.44960056022742</v>
       </c>
     </row>
-    <row r="90" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>4.1100000000000003</v>
       </c>
@@ -37240,7 +37565,7 @@
         <v>58.506699317644127</v>
       </c>
     </row>
-    <row r="91" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>-9.27</v>
       </c>
@@ -37647,7 +37972,7 @@
         <v>16.268600190545921</v>
       </c>
     </row>
-    <row r="92" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>7.68</v>
       </c>
@@ -38054,7 +38379,7 @@
         <v>206.90880006256208</v>
       </c>
     </row>
-    <row r="93" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>-9.18</v>
       </c>
@@ -38461,7 +38786,7 @@
         <v>419.27420492560083</v>
       </c>
     </row>
-    <row r="94" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>-2.68</v>
       </c>
@@ -38868,7 +39193,7 @@
         <v>113.61280088514819</v>
       </c>
     </row>
-    <row r="95" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>6.69</v>
       </c>
@@ -39275,7 +39600,7 @@
         <v>167.82990014081105</v>
       </c>
     </row>
-    <row r="96" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>-0.16</v>
       </c>
@@ -39682,7 +40007,7 @@
         <v>1.3247961733604341</v>
       </c>
     </row>
-    <row r="97" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>7.67</v>
       </c>
@@ -40089,7 +40414,7 @@
         <v>50.863299258685288</v>
       </c>
     </row>
-    <row r="98" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>-0.84</v>
       </c>
@@ -40496,7 +40821,7 @@
         <v>71.392001237150382</v>
       </c>
     </row>
-    <row r="99" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>-3.51</v>
       </c>
@@ -40903,7 +41228,7 @@
         <v>-45.230099879926421</v>
       </c>
     </row>
-    <row r="100" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>-6.29</v>
       </c>
@@ -41310,7 +41635,7 @@
         <v>85.319199244320458</v>
       </c>
     </row>
-    <row r="101" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2.46</v>
       </c>
@@ -41720,4 +42045,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8769910-DB2C-4DAB-8D65-FFF4713D77C9}">
+  <dimension ref="B3:N40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="B40:G40"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>